<commit_message>
Change X/Y_test to X/Y_train
</commit_message>
<xml_diff>
--- a/salida_with_features.xlsx
+++ b/salida_with_features.xlsx
@@ -432,11 +432,8 @@
           <t>LR</t>
         </is>
       </c>
-      <c r="C1" t="n">
-        <v>0.7831325301204819</v>
-      </c>
       <c r="D1" t="n">
-        <v>0.8855421686746988</v>
+        <v>0.7845659163987139</v>
       </c>
     </row>
     <row r="2">
@@ -450,11 +447,8 @@
           <t>KNN</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>0.7349397590361446</v>
-      </c>
       <c r="D2" t="n">
-        <v>0.8795180722891566</v>
+        <v>0.7154340836012861</v>
       </c>
     </row>
     <row r="3">
@@ -468,11 +462,8 @@
           <t>CART</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0.9967845659163987</v>
       </c>
     </row>
     <row r="4">
@@ -486,11 +477,8 @@
           <t>NB</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>0.8614457831325302</v>
-      </c>
       <c r="D4" t="n">
-        <v>0.8493975903614458</v>
+        <v>0.8697749196141479</v>
       </c>
     </row>
     <row r="5">
@@ -504,11 +492,8 @@
           <t>ANN</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0.2349397590361446</v>
-      </c>
       <c r="D5" t="n">
-        <v>0.7650602409638554</v>
+        <v>0.7893890675241158</v>
       </c>
     </row>
     <row r="6">
@@ -522,11 +507,8 @@
           <t>SVM</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>0.7650602409638554</v>
-      </c>
       <c r="D6" t="n">
-        <v>0.7771084337349398</v>
+        <v>0.6639871382636656</v>
       </c>
     </row>
     <row r="7">
@@ -540,11 +522,8 @@
           <t>LR</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>0.7630057803468208</v>
-      </c>
       <c r="D7" t="n">
-        <v>0.8786127167630058</v>
+        <v>0.8164556962025317</v>
       </c>
     </row>
     <row r="8">
@@ -558,11 +537,8 @@
           <t>KNN</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>0.7283236994219653</v>
-      </c>
       <c r="D8" t="n">
-        <v>0.8786127167630058</v>
+        <v>0.7009493670886076</v>
       </c>
     </row>
     <row r="9">
@@ -576,11 +552,8 @@
           <t>CART</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0.9778481012658228</v>
       </c>
     </row>
     <row r="10">
@@ -594,11 +567,8 @@
           <t>NB</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>0.8323699421965318</v>
-      </c>
       <c r="D10" t="n">
-        <v>0.8439306358381503</v>
+        <v>0.8987341772151899</v>
       </c>
     </row>
     <row r="11">
@@ -612,11 +582,8 @@
           <t>ANN</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>0.7514450867052023</v>
-      </c>
       <c r="D11" t="n">
-        <v>0.7514450867052023</v>
+        <v>0.7958860759493671</v>
       </c>
     </row>
     <row r="12">
@@ -630,11 +597,8 @@
           <t>SVM</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>0.7514450867052023</v>
-      </c>
       <c r="D12" t="n">
-        <v>0.7976878612716763</v>
+        <v>0.685126582278481</v>
       </c>
     </row>
     <row r="13">
@@ -648,11 +612,8 @@
           <t>LR</t>
         </is>
       </c>
-      <c r="C13" t="n">
-        <v>0.7821229050279329</v>
-      </c>
       <c r="D13" t="n">
-        <v>0.8379888268156425</v>
+        <v>0.817629179331307</v>
       </c>
     </row>
     <row r="14">
@@ -666,11 +627,8 @@
           <t>KNN</t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>0.8044692737430168</v>
-      </c>
       <c r="D14" t="n">
-        <v>0.888268156424581</v>
+        <v>0.6975683890577508</v>
       </c>
     </row>
     <row r="15">
@@ -684,11 +642,8 @@
           <t>CART</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>0.994413407821229</v>
-      </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0.9893617021276596</v>
       </c>
     </row>
     <row r="16">
@@ -702,11 +657,8 @@
           <t>NB</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>0.8770949720670391</v>
-      </c>
       <c r="D16" t="n">
-        <v>0.8100558659217877</v>
+        <v>0.9194528875379939</v>
       </c>
     </row>
     <row r="17">
@@ -720,11 +672,8 @@
           <t>ANN</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>0.770949720670391</v>
-      </c>
       <c r="D17" t="n">
-        <v>0.770949720670391</v>
+        <v>0.8024316109422492</v>
       </c>
     </row>
     <row r="18">
@@ -738,11 +687,8 @@
           <t>SVM</t>
         </is>
       </c>
-      <c r="C18" t="n">
-        <v>0.770949720670391</v>
-      </c>
       <c r="D18" t="n">
-        <v>0.770949720670391</v>
+        <v>0.6854103343465046</v>
       </c>
     </row>
     <row r="19">
@@ -756,11 +702,8 @@
           <t>LR</t>
         </is>
       </c>
-      <c r="C19" t="n">
-        <v>0.7894736842105263</v>
-      </c>
       <c r="D19" t="n">
-        <v>0.8789473684210526</v>
+        <v>0.7843137254901961</v>
       </c>
     </row>
     <row r="20">
@@ -774,11 +717,8 @@
           <t>KNN</t>
         </is>
       </c>
-      <c r="C20" t="n">
-        <v>0.7684210526315789</v>
-      </c>
       <c r="D20" t="n">
-        <v>0.9</v>
+        <v>0.6802413273001509</v>
       </c>
     </row>
     <row r="21">
@@ -792,11 +732,8 @@
           <t>CART</t>
         </is>
       </c>
-      <c r="C21" t="n">
-        <v>0.9947368421052631</v>
-      </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0.9653092006033183</v>
       </c>
     </row>
     <row r="22">
@@ -810,11 +747,8 @@
           <t>NB</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>0.7315789473684211</v>
-      </c>
       <c r="D22" t="n">
-        <v>0.8526315789473684</v>
+        <v>0.8929110105580694</v>
       </c>
     </row>
     <row r="23">
@@ -828,11 +762,8 @@
           <t>ANN</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>0.2789473684210526</v>
-      </c>
       <c r="D23" t="n">
-        <v>0.7736842105263158</v>
+        <v>0.7873303167420814</v>
       </c>
     </row>
     <row r="24">
@@ -846,11 +777,8 @@
           <t>SVM</t>
         </is>
       </c>
-      <c r="C24" t="n">
-        <v>0.7736842105263158</v>
-      </c>
       <c r="D24" t="n">
-        <v>0.8105263157894737</v>
+        <v>0.6892911010558069</v>
       </c>
     </row>
     <row r="25">
@@ -864,11 +792,8 @@
           <t>LR</t>
         </is>
       </c>
-      <c r="C25" t="n">
-        <v>0.7692307692307693</v>
-      </c>
       <c r="D25" t="n">
-        <v>0.8901098901098901</v>
+        <v>0.7966360856269113</v>
       </c>
     </row>
     <row r="26">
@@ -882,11 +807,8 @@
           <t>KNN</t>
         </is>
       </c>
-      <c r="C26" t="n">
-        <v>0.7252747252747253</v>
-      </c>
       <c r="D26" t="n">
-        <v>0.8736263736263736</v>
+        <v>0.7064220183486238</v>
       </c>
     </row>
     <row r="27">
@@ -900,11 +822,8 @@
           <t>CART</t>
         </is>
       </c>
-      <c r="C27" t="n">
-        <v>0.9945054945054945</v>
-      </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>0.9892966360856269</v>
       </c>
     </row>
     <row r="28">
@@ -918,11 +837,8 @@
           <t>NB</t>
         </is>
       </c>
-      <c r="C28" t="n">
-        <v>0.8076923076923077</v>
-      </c>
       <c r="D28" t="n">
-        <v>0.8461538461538461</v>
+        <v>0.8853211009174312</v>
       </c>
     </row>
     <row r="29">
@@ -936,11 +852,8 @@
           <t>ANN</t>
         </is>
       </c>
-      <c r="C29" t="n">
-        <v>0.7912087912087912</v>
-      </c>
       <c r="D29" t="n">
-        <v>0.7912087912087912</v>
+        <v>0.7920489296636085</v>
       </c>
     </row>
     <row r="30">
@@ -954,11 +867,8 @@
           <t>SVM</t>
         </is>
       </c>
-      <c r="C30" t="n">
-        <v>0.7912087912087912</v>
-      </c>
       <c r="D30" t="n">
-        <v>0.8296703296703297</v>
+        <v>0.6758409785932722</v>
       </c>
     </row>
     <row r="31">
@@ -972,11 +882,8 @@
           <t>LR</t>
         </is>
       </c>
-      <c r="C31" t="n">
-        <v>0.7877094972067039</v>
-      </c>
       <c r="D31" t="n">
-        <v>0.88268156424581</v>
+        <v>0.810126582278481</v>
       </c>
     </row>
     <row r="32">
@@ -990,11 +897,8 @@
           <t>KNN</t>
         </is>
       </c>
-      <c r="C32" t="n">
-        <v>0.7821229050279329</v>
-      </c>
       <c r="D32" t="n">
-        <v>0.8770949720670391</v>
+        <v>0.6930379746835443</v>
       </c>
     </row>
     <row r="33">
@@ -1008,11 +912,8 @@
           <t>CART</t>
         </is>
       </c>
-      <c r="C33" t="n">
-        <v>1</v>
-      </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>0.9762658227848101</v>
       </c>
     </row>
     <row r="34">
@@ -1026,11 +927,8 @@
           <t>NB</t>
         </is>
       </c>
-      <c r="C34" t="n">
-        <v>0.7486033519553073</v>
-      </c>
       <c r="D34" t="n">
-        <v>0.8491620111731844</v>
+        <v>0.8718354430379747</v>
       </c>
     </row>
     <row r="35">
@@ -1044,11 +942,8 @@
           <t>ANN</t>
         </is>
       </c>
-      <c r="C35" t="n">
-        <v>0.8268156424581006</v>
-      </c>
       <c r="D35" t="n">
-        <v>0.8268156424581006</v>
+        <v>0.8006329113924051</v>
       </c>
     </row>
     <row r="36">
@@ -1062,11 +957,8 @@
           <t>SVM</t>
         </is>
       </c>
-      <c r="C36" t="n">
-        <v>0.8268156424581006</v>
-      </c>
       <c r="D36" t="n">
-        <v>0.8324022346368715</v>
+        <v>0.6598101265822784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>